<commit_message>
add loop function for read and write into xlsx file
</commit_message>
<xml_diff>
--- a/rest+discharge.xlsx
+++ b/rest+discharge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="8328" windowHeight="3336"/>
+    <workbookView xWindow="612" yWindow="588" windowWidth="21792" windowHeight="8040"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>V</t>
   </si>
@@ -27,152 +27,15 @@
   <si>
     <t>WH</t>
   </si>
-  <si>
-    <t>mAh</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wh</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <charset val="136"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
@@ -184,188 +47,15 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -373,293 +63,20 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="42">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - 輔色1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - 輔色2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - 輔色3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - 輔色4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - 輔色5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - 輔色6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - 輔色1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - 輔色2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - 輔色3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - 輔色4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - 輔色5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - 輔色6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - 輔色1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - 輔色2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - 輔色3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - 輔色4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - 輔色5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - 輔色6" xfId="41" builtinId="52" customBuiltin="1"/>
+  <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="中等" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="合計" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="計算方式" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="連結的儲存格" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="備註" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="說明文字" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="輔色1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="輔色2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="輔色3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="輔色4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="輔色5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="輔色6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="標題" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="標題 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="標題 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="標題 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="標題 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="輸入" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="輸出" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="檢查儲存格" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="壞" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="警告文字" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -955,15 +372,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F384"/>
+  <dimension ref="A1:D384"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -976,14 +393,8 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>41.601999999999997</v>
       </c>
@@ -997,7 +408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>41.601999999999997</v>
       </c>
@@ -1011,7 +422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>41.601999999999997</v>
       </c>
@@ -1025,7 +436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>41.601999999999997</v>
       </c>
@@ -1039,7 +450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>41.601999999999997</v>
       </c>
@@ -1053,7 +464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>41.601999999999997</v>
       </c>
@@ -1067,7 +478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>41.601999999999997</v>
       </c>
@@ -1081,7 +492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>41.601999999999997</v>
       </c>
@@ -1095,7 +506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>41.601999999999997</v>
       </c>
@@ -1109,7 +520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>41.601999999999997</v>
       </c>
@@ -1123,7 +534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>41.601999999999997</v>
       </c>
@@ -1137,7 +548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>41.601999999999997</v>
       </c>
@@ -1151,7 +562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>39.521999999999998</v>
       </c>
@@ -1165,7 +576,7 @@
         <v>0.64066999999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>39.389000000000003</v>
       </c>
@@ -1179,7 +590,7 @@
         <v>1.44177</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>39.274999999999999</v>
       </c>
@@ -6346,7 +5757,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>